<commit_message>
Fixed navbar responsiveness for tablet devices
</commit_message>
<xml_diff>
--- a/comments.xlsx
+++ b/comments.xlsx
@@ -90,12 +90,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -122,6 +128,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +433,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,11 +454,13 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:2" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">

</xml_diff>